<commit_message>
better matrice and fix ai controller
</commit_message>
<xml_diff>
--- a/Ressources/Matrices.xlsx
+++ b/Ressources/Matrices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28706"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_1F250CBB5C9AD6D7F98DA79F1C411F4291579476" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5AE8D1E-48B4-44F3-A623-12C2727AB550}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_1F250CBB5C9AD6D7F98DA79F1C411F4291579476" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{162419D2-9E43-476C-9007-8A794D9CF5F9}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="28515" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,10 +144,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:8">

</xml_diff>